<commit_message>
idk what I´m doing
</commit_message>
<xml_diff>
--- a/logs/grind_stats.xlsx
+++ b/logs/grind_stats.xlsx
@@ -412,7 +412,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:S93"/>
+  <dimension ref="A1:S97"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
       <selection activeCell="A49" sqref="A49:XFD49"/>
@@ -6132,6 +6132,250 @@
         <v>0</v>
       </c>
     </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>2026-02-26 17:59:55</t>
+        </is>
+      </c>
+      <c r="B94" t="n">
+        <v>86344</v>
+      </c>
+      <c r="C94" t="n">
+        <v>102063</v>
+      </c>
+      <c r="D94" t="n">
+        <v>27752</v>
+      </c>
+      <c r="E94" t="n">
+        <v>50654</v>
+      </c>
+      <c r="F94" t="n">
+        <v>31079</v>
+      </c>
+      <c r="G94" t="n">
+        <v>17393</v>
+      </c>
+      <c r="H94" t="n">
+        <v>0</v>
+      </c>
+      <c r="I94" t="n">
+        <v>19136</v>
+      </c>
+      <c r="J94" t="n">
+        <v>55513</v>
+      </c>
+      <c r="K94" t="n">
+        <v>493</v>
+      </c>
+      <c r="L94" t="n">
+        <v>4438</v>
+      </c>
+      <c r="M94" t="n">
+        <v>0</v>
+      </c>
+      <c r="N94" t="n">
+        <v>0</v>
+      </c>
+      <c r="O94" t="n">
+        <v>151</v>
+      </c>
+      <c r="P94" t="n">
+        <v>172</v>
+      </c>
+      <c r="Q94" t="n">
+        <v>1800000</v>
+      </c>
+      <c r="R94" t="n">
+        <v>635335</v>
+      </c>
+      <c r="S94" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>2026-02-26 18:06:26</t>
+        </is>
+      </c>
+      <c r="B95" t="n">
+        <v>89575</v>
+      </c>
+      <c r="C95" t="n">
+        <v>106260</v>
+      </c>
+      <c r="D95" t="n">
+        <v>29014</v>
+      </c>
+      <c r="E95" t="n">
+        <v>52186</v>
+      </c>
+      <c r="F95" t="n">
+        <v>32087</v>
+      </c>
+      <c r="G95" t="n">
+        <v>17844</v>
+      </c>
+      <c r="H95" t="n">
+        <v>0</v>
+      </c>
+      <c r="I95" t="n">
+        <v>19752</v>
+      </c>
+      <c r="J95" t="n">
+        <v>57935</v>
+      </c>
+      <c r="K95" t="n">
+        <v>493</v>
+      </c>
+      <c r="L95" t="n">
+        <v>4633</v>
+      </c>
+      <c r="M95" t="n">
+        <v>0</v>
+      </c>
+      <c r="N95" t="n">
+        <v>0</v>
+      </c>
+      <c r="O95" t="n">
+        <v>152</v>
+      </c>
+      <c r="P95" t="n">
+        <v>173</v>
+      </c>
+      <c r="Q95" t="n">
+        <v>0</v>
+      </c>
+      <c r="R95" t="n">
+        <v>718754</v>
+      </c>
+      <c r="S95" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>2026-02-26 19:06:06</t>
+        </is>
+      </c>
+      <c r="B96" t="n">
+        <v>93343</v>
+      </c>
+      <c r="C96" t="n">
+        <v>111715</v>
+      </c>
+      <c r="D96" t="n">
+        <v>29834</v>
+      </c>
+      <c r="E96" t="n">
+        <v>53964</v>
+      </c>
+      <c r="F96" t="n">
+        <v>33585</v>
+      </c>
+      <c r="G96" t="n">
+        <v>18109</v>
+      </c>
+      <c r="H96" t="n">
+        <v>810</v>
+      </c>
+      <c r="I96" t="n">
+        <v>20639</v>
+      </c>
+      <c r="J96" t="n">
+        <v>60711</v>
+      </c>
+      <c r="K96" t="n">
+        <v>493</v>
+      </c>
+      <c r="L96" t="n">
+        <v>4870</v>
+      </c>
+      <c r="M96" t="n">
+        <v>0</v>
+      </c>
+      <c r="N96" t="n">
+        <v>0</v>
+      </c>
+      <c r="O96" t="n">
+        <v>154</v>
+      </c>
+      <c r="P96" t="n">
+        <v>175</v>
+      </c>
+      <c r="Q96" t="n">
+        <v>1800000</v>
+      </c>
+      <c r="R96" t="n">
+        <v>812874</v>
+      </c>
+      <c r="S96" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>2026-02-26 19:13:12</t>
+        </is>
+      </c>
+      <c r="B97" t="n">
+        <v>97420</v>
+      </c>
+      <c r="C97" t="n">
+        <v>115299</v>
+      </c>
+      <c r="D97" t="n">
+        <v>31307</v>
+      </c>
+      <c r="E97" t="n">
+        <v>56694</v>
+      </c>
+      <c r="F97" t="n">
+        <v>35051</v>
+      </c>
+      <c r="G97" t="n">
+        <v>19696</v>
+      </c>
+      <c r="H97" t="n">
+        <v>812</v>
+      </c>
+      <c r="I97" t="n">
+        <v>21489</v>
+      </c>
+      <c r="J97" t="n">
+        <v>62871</v>
+      </c>
+      <c r="K97" t="n">
+        <v>493</v>
+      </c>
+      <c r="L97" t="n">
+        <v>5135</v>
+      </c>
+      <c r="M97" t="n">
+        <v>0</v>
+      </c>
+      <c r="N97" t="n">
+        <v>0</v>
+      </c>
+      <c r="O97" t="n">
+        <v>154</v>
+      </c>
+      <c r="P97" t="n">
+        <v>176</v>
+      </c>
+      <c r="Q97" t="n">
+        <v>1800000</v>
+      </c>
+      <c r="R97" t="n">
+        <v>914296</v>
+      </c>
+      <c r="S97" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>